<commit_message>
profmat and pgmat at the xlsx
</commit_message>
<xml_diff>
--- a/lib/files/2018-1-Atualizada.xlsx
+++ b/lib/files/2018-1-Atualizada.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="205">
   <si>
     <t xml:space="preserve">COD_DISCIPLINA</t>
   </si>
@@ -545,16 +545,107 @@
   </si>
   <si>
     <t xml:space="preserve">INTRODUÇÃO À GEOMETRIA ANALÍTICA E ÁLGEBRA LINEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NÚMEROS E FUNÇÕES REAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATEMÁTICA DISCRETA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNDAMENTOS DE CÁLCULO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRABALHO DE CONCLUSÃO DE CURSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÁLGEBRA LINEAR APLICADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÁLGEBRA LINEAR AVANÇADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÁLGEBRA E MÓDULOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANÁLISE EM RN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQUAÇÕES DIFERENCIAIS PARCIAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIDA E INTEGRAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTIMIZAÇÃO I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEORIA DE DIST. E ANÁLISE DE FOURIER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -664,6 +755,34 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -727,7 +846,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -770,6 +889,113 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4C4C4C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF4C4C4C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4C4C4C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4C4C4C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4C4C4C"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -846,7 +1072,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -861,6 +1087,58 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -941,7 +1219,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF4C4C4C"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -956,13 +1234,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O240"/>
+  <dimension ref="A1:O257"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A227" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A249" activeCellId="0" sqref="240:249"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A221" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A258" activeCellId="0" sqref="A258"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.94"/>
@@ -12157,16 +12435,448 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C240" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D240" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E240" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G240" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I240" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L240" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D241" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F241" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G241" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I241" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L241" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D242" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E242" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F242" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G242" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I242" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L242" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D243" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E243" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F243" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G243" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I243" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L243" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B244" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D244" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E244" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F244" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G244" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I244" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="L244" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B245" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D245" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E245" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F245" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G245" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I245" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="L245" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B246" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D246" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E246" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F246" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G246" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I246" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L246" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B247" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D247" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E247" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F247" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G247" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I247" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L247" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B248" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D248" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E248" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F248" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G248" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I248" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L248" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B249" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D249" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E249" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F249" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G249" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I249" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="L249" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B250" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D250" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F250" s="16"/>
+      <c r="G250" s="16"/>
+      <c r="I250" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B251" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D251" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F251" s="16"/>
+      <c r="G251" s="16"/>
+      <c r="I251" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B252" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D252" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F252" s="16"/>
+      <c r="G252" s="16"/>
+      <c r="I252" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B253" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C253" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D253" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F253" s="16"/>
+      <c r="G253" s="16"/>
+      <c r="I253" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B254" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C254" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D254" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F254" s="16"/>
+      <c r="G254" s="16"/>
+      <c r="I254" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B255" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C255" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D255" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F255" s="16"/>
+      <c r="G255" s="16"/>
+      <c r="I255" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B256" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D256" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F256" s="16"/>
+      <c r="G256" s="16"/>
+      <c r="I256" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B257" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C257" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D257" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F257" s="16"/>
+      <c r="G257" s="16"/>
+      <c r="I257" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>